<commit_message>
- made that if virtual building stock service dwelling stock is driven by population - make that correct ey efficiency depending on GSHP_ASHP fraction is calculated and which is now loaded as a strategy variable
</commit_message>
<xml_diff>
--- a/config_data/scenario_and_base_data/efficiencies_definition.xlsx
+++ b/config_data/scenario_and_base_data/efficiencies_definition.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="13860" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="13860" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lighting" sheetId="1" r:id="rId1"/>
     <sheet name="Cooking" sheetId="2" r:id="rId2"/>
     <sheet name="Biomass CHP" sheetId="3" r:id="rId3"/>
     <sheet name="District heating" sheetId="4" r:id="rId4"/>
+    <sheet name="GSHP_ASHP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Calulating lighting efficiencies</t>
   </si>
@@ -110,6 +111,9 @@
   </si>
   <si>
     <t>Suggested connections</t>
+  </si>
+  <si>
+    <t>Staffel et al. 2012</t>
   </si>
 </sst>
 </file>
@@ -539,6 +543,66 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1323975" y="514350"/>
+          <a:ext cx="9972675" cy="4981575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1110,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1156,4 +1220,25 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>